<commit_message>
Challenge - Monday night submit
</commit_message>
<xml_diff>
--- a/Working/HW1_Working/1D ss satd_GEN.xlsx
+++ b/Working/HW1_Working/1D ss satd_GEN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\HWRS_582\hw-genoonan\Working\HW1_Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6067CF6A-C00F-493B-A49E-4482985671A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61648F4-6B39-45CD-B39E-DAFF26163BE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="2" r:id="rId1"/>
@@ -2022,37 +2022,37 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44.79038150065643</c:v>
+                  <c:v>44.790615159008773</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.580863126009369</c:v>
+                  <c:v>29.581282970020549</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.371474588565645</c:v>
+                  <c:v>14.372019066824675</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0064422224683778</c:v>
+                  <c:v>6.0069929991171582</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4856454815263129</c:v>
+                  <c:v>4.4861413649142756</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9649432054186309</c:v>
+                  <c:v>2.9653394300543767</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4443044504401066</c:v>
+                  <c:v>1.4445709225494243</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.60799492103578179</c:v>
+                  <c:v>0.60817023793708014</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45597264009878519</c:v>
+                  <c:v>0.45611528163551807</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30397390983983974</c:v>
+                  <c:v>0.30407272215124803</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.15198695491991987</c:v>
+                  <c:v>0.15203636107562402</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -2386,40 +2386,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>3.0419236998687139E-2</c:v>
+                  <c:v>3.0418769681982455E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0419036749294123E-2</c:v>
+                  <c:v>3.041866437797645E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0418777074887448E-2</c:v>
+                  <c:v>3.0418527806391746E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0418299513080969E-2</c:v>
+                  <c:v>3.0418276609845522E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0415934818841295E-2</c:v>
+                  <c:v>3.0417032684057654E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0414045522153644E-2</c:v>
+                  <c:v>3.0416038697197979E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0412775099570487E-2</c:v>
+                  <c:v>3.0415370150099048E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0411255614702717E-2</c:v>
+                  <c:v>3.0414570349539791E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0404456187399322E-2</c:v>
+                  <c:v>3.0410991260312416E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0399746051789089E-2</c:v>
+                  <c:v>3.0408511896854007E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0397390983983974E-2</c:v>
+                  <c:v>3.0407272215124802E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0397390983983974E-2</c:v>
+                  <c:v>3.0407272215124802E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4752,8 +4752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE611FA0-C15B-47E2-BD45-BA5083E6D7FE}">
   <dimension ref="B3:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:AB57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V52" sqref="V52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5459,8 +5459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5791BB39-6ADA-49F6-933B-F3F429707484}">
   <dimension ref="B3:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI26" sqref="AI26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5625,11 +5625,11 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" ref="I9:I19" ca="1" si="0">(I8*2/(1/H8+1/H9)+I10*2/(1/H9+1/H10))/(2/(1/H8+1/H9)+2/(1/H9+1/H10))</f>
-        <v>44.79038150065643</v>
+        <v>44.790615159008773</v>
       </c>
       <c r="J9" s="25">
         <f ca="1">(I8-I9)/inputs!$D$8*2/(1/H8+1/H9)</f>
-        <v>3.0419236998687139E-2</v>
+        <v>3.0418769681982455E-2</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:L20" si="1">IF($G9=1,1,0)</f>
@@ -5671,11 +5671,11 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>29.580863126009369</v>
+        <v>29.581282970020549</v>
       </c>
       <c r="J10" s="25">
         <f ca="1">(I9-I10)/inputs!$D$8*2/(1/H9+1/H10)</f>
-        <v>3.0419036749294123E-2</v>
+        <v>3.041866437797645E-2</v>
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
@@ -5722,11 +5722,11 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>14.371474588565645</v>
+        <v>14.372019066824675</v>
       </c>
       <c r="J11" s="25">
         <f ca="1">(I10-I11)/inputs!$D$8*2/(1/H10+1/H11)</f>
-        <v>3.0418777074887448E-2</v>
+        <v>3.0418527806391746E-2</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
@@ -5772,11 +5772,11 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0064422224683778</v>
+        <v>6.0069929991171582</v>
       </c>
       <c r="J12" s="25">
         <f ca="1">(I11-I12)/inputs!$D$8*2/(1/H11+1/H12)</f>
-        <v>3.0418299513080969E-2</v>
+        <v>3.0418276609845522E-2</v>
       </c>
       <c r="L12">
         <f t="shared" si="1"/>
@@ -5814,11 +5814,11 @@
       </c>
       <c r="I13" s="1">
         <f ca="1">(I12*2/(1/H12+1/H13)+I14*2/(1/H13+1/H14))/(2/(1/H12+1/H13)+2/(1/H13+1/H14))</f>
-        <v>4.4856454815263129</v>
+        <v>4.4861413649142756</v>
       </c>
       <c r="J13" s="25">
         <f ca="1">(I12-I13)/inputs!$D$8*2/(1/H12+1/H13)</f>
-        <v>3.0415934818841295E-2</v>
+        <v>3.0417032684057654E-2</v>
       </c>
       <c r="L13">
         <f t="shared" si="1"/>
@@ -5856,11 +5856,11 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9649432054186309</v>
+        <v>2.9653394300543767</v>
       </c>
       <c r="J14" s="25">
         <f ca="1">(I13-I14)/inputs!$D$8*2/(1/H13+1/H14)</f>
-        <v>3.0414045522153644E-2</v>
+        <v>3.0416038697197979E-2</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
@@ -5898,11 +5898,11 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4443044504401066</v>
+        <v>1.4445709225494243</v>
       </c>
       <c r="J15" s="25">
         <f ca="1">(I14-I15)/inputs!$D$8*2/(1/H14+1/H15)</f>
-        <v>3.0412775099570487E-2</v>
+        <v>3.0415370150099048E-2</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
@@ -5940,11 +5940,11 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60799492103578179</v>
+        <v>0.60817023793708014</v>
       </c>
       <c r="J16" s="25">
         <f ca="1">(I15-I16)/inputs!$D$8*2/(1/H15+1/H16)</f>
-        <v>3.0411255614702717E-2</v>
+        <v>3.0414570349539791E-2</v>
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
@@ -5982,11 +5982,11 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45597264009878519</v>
+        <v>0.45611528163551807</v>
       </c>
       <c r="J17" s="25">
         <f ca="1">(I16-I17)/inputs!$D$8*2/(1/H16+1/H17)</f>
-        <v>3.0404456187399322E-2</v>
+        <v>3.0410991260312416E-2</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
@@ -6024,11 +6024,11 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30397390983983974</v>
+        <v>0.30407272215124803</v>
       </c>
       <c r="J18" s="25">
         <f ca="1">(I17-I18)/inputs!$D$8*2/(1/H17+1/H18)</f>
-        <v>3.0399746051789089E-2</v>
+        <v>3.0408511896854007E-2</v>
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
@@ -6066,11 +6066,11 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15198695491991987</v>
+        <v>0.15203636107562402</v>
       </c>
       <c r="J19" s="25">
         <f ca="1">(I18-I19)/inputs!$D$8*2/(1/H18+1/H19)</f>
-        <v>3.0397390983983974E-2</v>
+        <v>3.0407272215124802E-2</v>
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
@@ -6111,7 +6111,7 @@
       </c>
       <c r="J20" s="25">
         <f ca="1">(I19-I20)/inputs!$D$8*2/(1/H19+1/H20)</f>
-        <v>3.0397390983983974E-2</v>
+        <v>3.0407272215124802E-2</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>

</xml_diff>